<commit_message>
Penyempurnaan input kinerja SIOD, tambah manual, Insya Allah kinerja beres
</commit_message>
<xml_diff>
--- a/coba - Copy.xlsx
+++ b/coba - Copy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19020" windowHeight="9345" tabRatio="961" activeTab="10"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19020" windowHeight="9345" tabRatio="961" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Operasi Harian" sheetId="1" r:id="rId1"/>
@@ -5378,7 +5378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
@@ -33839,8 +33839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD88"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
revisi klasifikasi 41 dan perhitungan performansi dari madiun
</commit_message>
<xml_diff>
--- a/coba - Copy.xlsx
+++ b/coba - Copy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19020" windowHeight="9345" tabRatio="961" activeTab="10"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19020" windowHeight="9345" tabRatio="961" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Operasi Harian" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2557" uniqueCount="603">
   <si>
     <t>PT. Patra Niaga</t>
   </si>
@@ -3111,7 +3111,7 @@
     <xf numFmtId="165" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="25" fillId="34" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3240,6 +3240,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="54" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="27" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3701,8 +3705,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A1" s="77"/>
-      <c r="B1" s="77"/>
+      <c r="A1" s="78"/>
+      <c r="B1" s="78"/>
     </row>
     <row r="2" spans="1:31" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
@@ -3791,15 +3795,15 @@
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="78">
+      <c r="F6" s="79">
         <v>41761</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="11"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -3837,15 +3841,15 @@
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="78">
+      <c r="F8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="11"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -4244,15 +4248,15 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="78">
+      <c r="F6" s="79">
         <v>41761</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -4270,15 +4274,15 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>528</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="78">
+      <c r="F8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -4336,8 +4340,8 @@
       <c r="I13" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="J13" s="84"/>
-      <c r="K13" s="81"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="82"/>
     </row>
     <row r="14" spans="1:11" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -5400,10 +5404,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5415,12 +5419,10 @@
     <col min="5" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
     <col min="8" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="3.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" customWidth="1"/>
+    <col min="10" max="11" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
@@ -5429,7 +5431,7 @@
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
-    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -5442,7 +5444,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -5451,7 +5453,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -5460,7 +5462,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
       <c r="C5" s="12" t="s">
         <v>2</v>
@@ -5473,20 +5475,20 @@
       <c r="G5" s="10"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="78">
+      <c r="F6" s="79">
         <v>41761</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="9"/>
       <c r="C7" s="13" t="s">
         <v>5</v>
@@ -5499,20 +5501,20 @@
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>565</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="78">
+      <c r="F8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="13"/>
@@ -5521,7 +5523,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -5530,7 +5532,7 @@
       <c r="G10" s="18"/>
       <c r="H10" s="19"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -5539,7 +5541,7 @@
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
     </row>
-    <row r="13" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -5570,10 +5572,11 @@
       <c r="J13" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="K13" s="84"/>
-      <c r="L13" s="81"/>
-    </row>
-    <row r="14" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K13" s="77" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -5593,7 +5596,7 @@
         <v>476</v>
       </c>
       <c r="G14" s="42">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="H14" s="42">
         <v>202</v>
@@ -5604,14 +5607,11 @@
       <c r="J14" s="42">
         <v>1</v>
       </c>
-      <c r="K14" s="47" t="s">
-        <v>455</v>
-      </c>
-      <c r="L14" s="48">
-        <v>84069</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -5642,14 +5642,11 @@
       <c r="J15">
         <v>2</v>
       </c>
-      <c r="K15" s="45" t="s">
-        <v>455</v>
-      </c>
-      <c r="L15" s="46">
-        <v>160007</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -5680,14 +5677,11 @@
       <c r="J16" s="42">
         <v>2</v>
       </c>
-      <c r="K16" s="47" t="s">
-        <v>455</v>
-      </c>
-      <c r="L16" s="48">
-        <v>108652</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K16" s="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -5718,19 +5712,14 @@
       <c r="J17">
         <v>2</v>
       </c>
-      <c r="K17" s="45" t="s">
-        <v>455</v>
-      </c>
-      <c r="L17" s="46">
-        <v>127814</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="43"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="46"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" s="44"/>
       <c r="C19" s="42"/>
       <c r="D19" s="42"/>
@@ -5740,15 +5729,12 @@
       <c r="H19" s="42"/>
       <c r="I19" s="42"/>
       <c r="J19" s="42"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="48"/>
-    </row>
-    <row r="20" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K19" s="42"/>
+    </row>
+    <row r="20" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="43"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="46"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" s="44"/>
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
@@ -5758,15 +5744,12 @@
       <c r="H21" s="42"/>
       <c r="I21" s="42"/>
       <c r="J21" s="42"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="48"/>
-    </row>
-    <row r="22" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K21" s="42"/>
+    </row>
+    <row r="22" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="43"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="46"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" s="44"/>
       <c r="C23" s="42"/>
       <c r="D23" s="42"/>
@@ -5776,15 +5759,12 @@
       <c r="H23" s="42"/>
       <c r="I23" s="42"/>
       <c r="J23" s="42"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="48"/>
-    </row>
-    <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K23" s="42"/>
+    </row>
+    <row r="24" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="43"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="46"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B25" s="44"/>
       <c r="C25" s="42"/>
       <c r="D25" s="42"/>
@@ -5794,15 +5774,12 @@
       <c r="H25" s="42"/>
       <c r="I25" s="42"/>
       <c r="J25" s="42"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="48"/>
-    </row>
-    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K25" s="42"/>
+    </row>
+    <row r="26" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="43"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="46"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B27" s="44"/>
       <c r="C27" s="42"/>
       <c r="D27" s="42"/>
@@ -5812,15 +5789,12 @@
       <c r="H27" s="42"/>
       <c r="I27" s="42"/>
       <c r="J27" s="42"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="48"/>
-    </row>
-    <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K27" s="42"/>
+    </row>
+    <row r="28" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="43"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="46"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B29" s="44"/>
       <c r="C29" s="42"/>
       <c r="D29" s="42"/>
@@ -5830,15 +5804,12 @@
       <c r="H29" s="42"/>
       <c r="I29" s="42"/>
       <c r="J29" s="42"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="48"/>
-    </row>
-    <row r="30" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K29" s="42"/>
+    </row>
+    <row r="30" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="43"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="46"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B31" s="44"/>
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
@@ -5848,15 +5819,12 @@
       <c r="H31" s="42"/>
       <c r="I31" s="42"/>
       <c r="J31" s="42"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="48"/>
-    </row>
-    <row r="32" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K31" s="42"/>
+    </row>
+    <row r="32" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="43"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="46"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="44"/>
       <c r="C33" s="42"/>
       <c r="D33" s="42"/>
@@ -5866,15 +5834,12 @@
       <c r="H33" s="42"/>
       <c r="I33" s="42"/>
       <c r="J33" s="42"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="48"/>
-    </row>
-    <row r="34" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K33" s="42"/>
+    </row>
+    <row r="34" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="43"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="46"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="44"/>
       <c r="C35" s="42"/>
       <c r="D35" s="42"/>
@@ -5884,15 +5849,12 @@
       <c r="H35" s="42"/>
       <c r="I35" s="42"/>
       <c r="J35" s="42"/>
-      <c r="K35" s="47"/>
-      <c r="L35" s="48"/>
-    </row>
-    <row r="36" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K35" s="42"/>
+    </row>
+    <row r="36" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="43"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="46"/>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="44"/>
       <c r="C37" s="42"/>
       <c r="D37" s="42"/>
@@ -5902,15 +5864,12 @@
       <c r="H37" s="42"/>
       <c r="I37" s="42"/>
       <c r="J37" s="42"/>
-      <c r="K37" s="47"/>
-      <c r="L37" s="48"/>
-    </row>
-    <row r="38" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K37" s="42"/>
+    </row>
+    <row r="38" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="43"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="46"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39" s="44"/>
       <c r="C39" s="42"/>
       <c r="D39" s="42"/>
@@ -5920,15 +5879,12 @@
       <c r="H39" s="42"/>
       <c r="I39" s="42"/>
       <c r="J39" s="42"/>
-      <c r="K39" s="47"/>
-      <c r="L39" s="48"/>
-    </row>
-    <row r="40" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K39" s="42"/>
+    </row>
+    <row r="40" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="43"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="46"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41" s="44"/>
       <c r="C41" s="42"/>
       <c r="D41" s="42"/>
@@ -5938,15 +5894,12 @@
       <c r="H41" s="42"/>
       <c r="I41" s="42"/>
       <c r="J41" s="42"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="48"/>
-    </row>
-    <row r="42" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K41" s="42"/>
+    </row>
+    <row r="42" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="43"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="46"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B43" s="44"/>
       <c r="C43" s="42"/>
       <c r="D43" s="42"/>
@@ -5956,15 +5909,12 @@
       <c r="H43" s="42"/>
       <c r="I43" s="42"/>
       <c r="J43" s="42"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="48"/>
-    </row>
-    <row r="44" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K43" s="42"/>
+    </row>
+    <row r="44" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="43"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="46"/>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="44"/>
       <c r="C45" s="42"/>
       <c r="D45" s="42"/>
@@ -5974,15 +5924,12 @@
       <c r="H45" s="42"/>
       <c r="I45" s="42"/>
       <c r="J45" s="42"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="48"/>
-    </row>
-    <row r="46" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K45" s="42"/>
+    </row>
+    <row r="46" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="43"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="46"/>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="44"/>
       <c r="C47" s="42"/>
       <c r="D47" s="42"/>
@@ -5992,15 +5939,12 @@
       <c r="H47" s="42"/>
       <c r="I47" s="42"/>
       <c r="J47" s="42"/>
-      <c r="K47" s="47"/>
-      <c r="L47" s="48"/>
-    </row>
-    <row r="48" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K47" s="42"/>
+    </row>
+    <row r="48" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="43"/>
-      <c r="K48" s="45"/>
-      <c r="L48" s="46"/>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B49" s="44"/>
       <c r="C49" s="42"/>
       <c r="D49" s="42"/>
@@ -6010,15 +5954,12 @@
       <c r="H49" s="42"/>
       <c r="I49" s="42"/>
       <c r="J49" s="42"/>
-      <c r="K49" s="47"/>
-      <c r="L49" s="48"/>
-    </row>
-    <row r="50" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K49" s="42"/>
+    </row>
+    <row r="50" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="43"/>
-      <c r="K50" s="45"/>
-      <c r="L50" s="46"/>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B51" s="44"/>
       <c r="C51" s="42"/>
       <c r="D51" s="42"/>
@@ -6028,15 +5969,12 @@
       <c r="H51" s="42"/>
       <c r="I51" s="42"/>
       <c r="J51" s="42"/>
-      <c r="K51" s="47"/>
-      <c r="L51" s="48"/>
-    </row>
-    <row r="52" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K51" s="42"/>
+    </row>
+    <row r="52" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="43"/>
-      <c r="K52" s="45"/>
-      <c r="L52" s="46"/>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B53" s="44"/>
       <c r="C53" s="42"/>
       <c r="D53" s="42"/>
@@ -6046,15 +5984,12 @@
       <c r="H53" s="42"/>
       <c r="I53" s="42"/>
       <c r="J53" s="42"/>
-      <c r="K53" s="47"/>
-      <c r="L53" s="48"/>
-    </row>
-    <row r="54" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K53" s="42"/>
+    </row>
+    <row r="54" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="43"/>
-      <c r="K54" s="45"/>
-      <c r="L54" s="46"/>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B55" s="44"/>
       <c r="C55" s="42"/>
       <c r="D55" s="42"/>
@@ -6064,15 +5999,12 @@
       <c r="H55" s="42"/>
       <c r="I55" s="42"/>
       <c r="J55" s="42"/>
-      <c r="K55" s="47"/>
-      <c r="L55" s="48"/>
-    </row>
-    <row r="56" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K55" s="42"/>
+    </row>
+    <row r="56" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="43"/>
-      <c r="K56" s="45"/>
-      <c r="L56" s="46"/>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B57" s="44"/>
       <c r="C57" s="42"/>
       <c r="D57" s="42"/>
@@ -6082,15 +6014,12 @@
       <c r="H57" s="42"/>
       <c r="I57" s="42"/>
       <c r="J57" s="42"/>
-      <c r="K57" s="47"/>
-      <c r="L57" s="48"/>
-    </row>
-    <row r="58" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K57" s="42"/>
+    </row>
+    <row r="58" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="43"/>
-      <c r="K58" s="45"/>
-      <c r="L58" s="46"/>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B59" s="44"/>
       <c r="C59" s="42"/>
       <c r="D59" s="42"/>
@@ -6100,15 +6029,12 @@
       <c r="H59" s="42"/>
       <c r="I59" s="42"/>
       <c r="J59" s="42"/>
-      <c r="K59" s="47"/>
-      <c r="L59" s="48"/>
-    </row>
-    <row r="60" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K59" s="42"/>
+    </row>
+    <row r="60" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="43"/>
-      <c r="K60" s="45"/>
-      <c r="L60" s="46"/>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B61" s="44"/>
       <c r="C61" s="42"/>
       <c r="D61" s="42"/>
@@ -6118,15 +6044,12 @@
       <c r="H61" s="42"/>
       <c r="I61" s="42"/>
       <c r="J61" s="42"/>
-      <c r="K61" s="47"/>
-      <c r="L61" s="48"/>
-    </row>
-    <row r="62" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K61" s="42"/>
+    </row>
+    <row r="62" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="43"/>
-      <c r="K62" s="45"/>
-      <c r="L62" s="46"/>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B63" s="44"/>
       <c r="C63" s="42"/>
       <c r="D63" s="42"/>
@@ -6136,15 +6059,12 @@
       <c r="H63" s="42"/>
       <c r="I63" s="42"/>
       <c r="J63" s="42"/>
-      <c r="K63" s="47"/>
-      <c r="L63" s="48"/>
-    </row>
-    <row r="64" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K63" s="42"/>
+    </row>
+    <row r="64" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="43"/>
-      <c r="K64" s="45"/>
-      <c r="L64" s="46"/>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B65" s="44"/>
       <c r="C65" s="42"/>
       <c r="D65" s="42"/>
@@ -6154,15 +6074,12 @@
       <c r="H65" s="42"/>
       <c r="I65" s="42"/>
       <c r="J65" s="42"/>
-      <c r="K65" s="47"/>
-      <c r="L65" s="48"/>
-    </row>
-    <row r="66" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K65" s="42"/>
+    </row>
+    <row r="66" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="43"/>
-      <c r="K66" s="45"/>
-      <c r="L66" s="46"/>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B67" s="44"/>
       <c r="C67" s="42"/>
       <c r="D67" s="42"/>
@@ -6172,15 +6089,12 @@
       <c r="H67" s="42"/>
       <c r="I67" s="42"/>
       <c r="J67" s="42"/>
-      <c r="K67" s="47"/>
-      <c r="L67" s="48"/>
-    </row>
-    <row r="68" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K67" s="42"/>
+    </row>
+    <row r="68" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="43"/>
-      <c r="K68" s="45"/>
-      <c r="L68" s="46"/>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B69" s="44"/>
       <c r="C69" s="42"/>
       <c r="D69" s="42"/>
@@ -6190,17 +6104,15 @@
       <c r="H69" s="42"/>
       <c r="I69" s="42"/>
       <c r="J69" s="42"/>
-      <c r="K69" s="47"/>
-      <c r="L69" s="48"/>
+      <c r="K69" s="42"/>
     </row>
   </sheetData>
   <sheetProtection objects="1" scenarios="1"/>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="K13:L13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6315,10 +6227,10 @@
       </c>
       <c r="E6" s="55"/>
       <c r="F6" s="55"/>
-      <c r="G6" s="78">
+      <c r="G6" s="79">
         <v>41761</v>
       </c>
-      <c r="H6" s="79"/>
+      <c r="H6" s="80"/>
       <c r="I6" s="11"/>
       <c r="J6" s="55"/>
       <c r="K6" s="55"/>
@@ -6351,10 +6263,10 @@
       </c>
       <c r="E8" s="55"/>
       <c r="F8" s="55"/>
-      <c r="G8" s="78">
+      <c r="G8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="H8" s="79"/>
+      <c r="H8" s="80"/>
       <c r="I8" s="11"/>
       <c r="J8" s="55"/>
       <c r="K8" s="55"/>
@@ -6381,16 +6293,16 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="63"/>
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="88" t="s">
         <v>568</v>
       </c>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="88" t="s">
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="89" t="s">
         <v>569</v>
       </c>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
       <c r="H13" s="64"/>
       <c r="I13" s="64"/>
       <c r="J13" s="64"/>
@@ -6791,16 +6703,16 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="63"/>
-      <c r="B26" s="89" t="s">
+      <c r="B26" s="90" t="s">
         <v>579</v>
       </c>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="90" t="s">
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="91" t="s">
         <v>569</v>
       </c>
-      <c r="F26" s="90"/>
-      <c r="G26" s="90"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="91"/>
       <c r="H26" s="70"/>
       <c r="I26" s="70"/>
       <c r="J26" s="70"/>
@@ -7203,15 +7115,15 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="63"/>
-      <c r="B39" s="85" t="s">
+      <c r="B39" s="86" t="s">
         <v>581</v>
       </c>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="86" t="s">
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="87" t="s">
         <v>582</v>
       </c>
-      <c r="F39" s="86"/>
+      <c r="F39" s="87"/>
       <c r="G39" s="71"/>
       <c r="H39" s="71"/>
       <c r="I39" s="71"/>
@@ -7906,15 +7818,15 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="78">
+      <c r="F6" s="79">
         <v>41761</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -7932,15 +7844,15 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="78">
+      <c r="F8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -7971,21 +7883,21 @@
       <c r="H11" s="20"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="83"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="84"/>
     </row>
     <row r="14" spans="1:8" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="80"/>
-      <c r="D14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="82"/>
       <c r="E14" s="22" t="s">
         <v>44</v>
       </c>
@@ -8259,16 +8171,16 @@
       <c r="A29" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="80" t="s">
+      <c r="B29" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="80"/>
-      <c r="D29" s="81"/>
+      <c r="C29" s="81"/>
+      <c r="D29" s="82"/>
       <c r="E29" s="22"/>
-      <c r="F29" s="80" t="s">
+      <c r="F29" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="G29" s="81"/>
+      <c r="G29" s="82"/>
     </row>
     <row r="30" spans="1:7" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27" t="s">
@@ -8387,17 +8299,17 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="27"/>
-      <c r="B37" s="82"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
     </row>
     <row r="38" spans="1:7" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="27"/>
-      <c r="B38" s="80" t="s">
+      <c r="B38" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="81"/>
+      <c r="C38" s="82"/>
       <c r="D38" s="22" t="s">
         <v>75</v>
       </c>
@@ -8539,15 +8451,15 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="78">
+      <c r="F6" s="79">
         <v>41761</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -8565,15 +8477,15 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="78">
+      <c r="F8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -13302,15 +13214,15 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="78">
+      <c r="F6" s="79">
         <v>41761</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -13328,15 +13240,15 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>219</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="78">
+      <c r="F8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -18660,15 +18572,15 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="78">
+      <c r="F6" s="79">
         <v>41761</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -18686,15 +18598,15 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>222</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="78">
+      <c r="F8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -24628,15 +24540,15 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="78">
+      <c r="F6" s="79">
         <v>41761</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
@@ -24654,15 +24566,15 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>357</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="78">
+      <c r="F8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
@@ -31716,15 +31628,15 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="78">
+      <c r="F6" s="79">
         <v>41761</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
@@ -31742,15 +31654,15 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>439</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="78">
+      <c r="F8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.2">
@@ -33632,15 +33544,15 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="78">
+      <c r="F6" s="79">
         <v>41761</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -33658,15 +33570,15 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>445</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="78">
+      <c r="F8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -33724,10 +33636,10 @@
       <c r="I13" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="J13" s="84" t="s">
+      <c r="J13" s="85" t="s">
         <v>451</v>
       </c>
-      <c r="K13" s="81"/>
+      <c r="K13" s="82"/>
     </row>
     <row r="14" spans="1:11" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -34637,10 +34549,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -34652,12 +34564,10 @@
     <col min="5" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
     <col min="8" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="3.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" customWidth="1"/>
+    <col min="10" max="11" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
@@ -34666,7 +34576,7 @@
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
-    <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -34679,7 +34589,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -34688,7 +34598,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -34697,7 +34607,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
       <c r="C5" s="12" t="s">
         <v>2</v>
@@ -34710,20 +34620,20 @@
       <c r="G5" s="10"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="79"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="78">
+      <c r="F6" s="79">
         <v>41761</v>
       </c>
-      <c r="G6" s="79"/>
+      <c r="G6" s="80"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="9"/>
       <c r="C7" s="13" t="s">
         <v>5</v>
@@ -34736,20 +34646,20 @@
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
-      <c r="C8" s="78" t="s">
+      <c r="C8" s="79" t="s">
         <v>527</v>
       </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="78">
+      <c r="F8" s="79">
         <v>41761.999988425923</v>
       </c>
-      <c r="G8" s="79"/>
+      <c r="G8" s="80"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="13"/>
@@ -34758,7 +34668,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -34767,7 +34677,7 @@
       <c r="G10" s="18"/>
       <c r="H10" s="19"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -34776,7 +34686,7 @@
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
     </row>
-    <row r="13" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -34807,12 +34717,11 @@
       <c r="J13" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="K13" s="84" t="s">
-        <v>451</v>
-      </c>
-      <c r="L13" s="81"/>
-    </row>
-    <row r="14" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K13" s="77" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -34832,7 +34741,7 @@
         <v>454</v>
       </c>
       <c r="G14" s="42">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="H14" s="42">
         <v>245</v>
@@ -34843,14 +34752,11 @@
       <c r="J14" s="42">
         <v>2</v>
       </c>
-      <c r="K14" s="47" t="s">
-        <v>455</v>
-      </c>
-      <c r="L14" s="48">
-        <v>110103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -34881,14 +34787,11 @@
       <c r="J15">
         <v>2</v>
       </c>
-      <c r="K15" s="45" t="s">
-        <v>455</v>
-      </c>
-      <c r="L15" s="46">
-        <v>62288</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -34919,14 +34822,11 @@
       <c r="J16" s="42">
         <v>2</v>
       </c>
-      <c r="K16" s="47" t="s">
-        <v>455</v>
-      </c>
-      <c r="L16" s="48">
-        <v>87189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K16" s="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -34957,14 +34857,11 @@
       <c r="J17">
         <v>2</v>
       </c>
-      <c r="K17" s="45" t="s">
-        <v>455</v>
-      </c>
-      <c r="L17" s="46">
-        <v>105293</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B18" s="44"/>
       <c r="C18" s="42"/>
       <c r="D18" s="42"/>
@@ -34974,15 +34871,12 @@
       <c r="H18" s="42"/>
       <c r="I18" s="42"/>
       <c r="J18" s="42"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="48"/>
-    </row>
-    <row r="19" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K18" s="42"/>
+    </row>
+    <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="43"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="46"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="44"/>
       <c r="C20" s="42"/>
       <c r="D20" s="42"/>
@@ -34992,15 +34886,12 @@
       <c r="H20" s="42"/>
       <c r="I20" s="42"/>
       <c r="J20" s="42"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="48"/>
-    </row>
-    <row r="21" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K20" s="42"/>
+    </row>
+    <row r="21" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="43"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="46"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" s="44"/>
       <c r="C22" s="42"/>
       <c r="D22" s="42"/>
@@ -35010,15 +34901,12 @@
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
       <c r="J22" s="42"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="48"/>
-    </row>
-    <row r="23" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K22" s="42"/>
+    </row>
+    <row r="23" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="43"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="46"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24" s="44"/>
       <c r="C24" s="42"/>
       <c r="D24" s="42"/>
@@ -35028,15 +34916,12 @@
       <c r="H24" s="42"/>
       <c r="I24" s="42"/>
       <c r="J24" s="42"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="48"/>
-    </row>
-    <row r="25" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K24" s="42"/>
+    </row>
+    <row r="25" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="43"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="46"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26" s="44"/>
       <c r="C26" s="42"/>
       <c r="D26" s="42"/>
@@ -35046,15 +34931,12 @@
       <c r="H26" s="42"/>
       <c r="I26" s="42"/>
       <c r="J26" s="42"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="48"/>
-    </row>
-    <row r="27" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K26" s="42"/>
+    </row>
+    <row r="27" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="43"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="46"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B28" s="44"/>
       <c r="C28" s="42"/>
       <c r="D28" s="42"/>
@@ -35064,15 +34946,12 @@
       <c r="H28" s="42"/>
       <c r="I28" s="42"/>
       <c r="J28" s="42"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="48"/>
-    </row>
-    <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K28" s="42"/>
+    </row>
+    <row r="29" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="43"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="46"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B30" s="44"/>
       <c r="C30" s="42"/>
       <c r="D30" s="42"/>
@@ -35082,15 +34961,12 @@
       <c r="H30" s="42"/>
       <c r="I30" s="42"/>
       <c r="J30" s="42"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="48"/>
-    </row>
-    <row r="31" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K30" s="42"/>
+    </row>
+    <row r="31" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="43"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="46"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B32" s="44"/>
       <c r="C32" s="42"/>
       <c r="D32" s="42"/>
@@ -35100,15 +34976,12 @@
       <c r="H32" s="42"/>
       <c r="I32" s="42"/>
       <c r="J32" s="42"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="48"/>
-    </row>
-    <row r="33" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K32" s="42"/>
+    </row>
+    <row r="33" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="43"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="46"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="44"/>
       <c r="C34" s="42"/>
       <c r="D34" s="42"/>
@@ -35118,15 +34991,12 @@
       <c r="H34" s="42"/>
       <c r="I34" s="42"/>
       <c r="J34" s="42"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="48"/>
-    </row>
-    <row r="35" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K34" s="42"/>
+    </row>
+    <row r="35" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="43"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="46"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="44"/>
       <c r="C36" s="42"/>
       <c r="D36" s="42"/>
@@ -35136,15 +35006,12 @@
       <c r="H36" s="42"/>
       <c r="I36" s="42"/>
       <c r="J36" s="42"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="48"/>
-    </row>
-    <row r="37" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K36" s="42"/>
+    </row>
+    <row r="37" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="43"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="46"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="44"/>
       <c r="C38" s="42"/>
       <c r="D38" s="42"/>
@@ -35154,15 +35021,12 @@
       <c r="H38" s="42"/>
       <c r="I38" s="42"/>
       <c r="J38" s="42"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="48"/>
-    </row>
-    <row r="39" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K38" s="42"/>
+    </row>
+    <row r="39" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="43"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="46"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B40" s="44"/>
       <c r="C40" s="42"/>
       <c r="D40" s="42"/>
@@ -35172,15 +35036,12 @@
       <c r="H40" s="42"/>
       <c r="I40" s="42"/>
       <c r="J40" s="42"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="48"/>
-    </row>
-    <row r="41" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K40" s="42"/>
+    </row>
+    <row r="41" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="43"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="46"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B42" s="44"/>
       <c r="C42" s="42"/>
       <c r="D42" s="42"/>
@@ -35190,15 +35051,12 @@
       <c r="H42" s="42"/>
       <c r="I42" s="42"/>
       <c r="J42" s="42"/>
-      <c r="K42" s="47"/>
-      <c r="L42" s="48"/>
-    </row>
-    <row r="43" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K42" s="42"/>
+    </row>
+    <row r="43" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="43"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="46"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B44" s="44"/>
       <c r="C44" s="42"/>
       <c r="D44" s="42"/>
@@ -35208,15 +35066,12 @@
       <c r="H44" s="42"/>
       <c r="I44" s="42"/>
       <c r="J44" s="42"/>
-      <c r="K44" s="47"/>
-      <c r="L44" s="48"/>
-    </row>
-    <row r="45" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K44" s="42"/>
+    </row>
+    <row r="45" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="43"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="46"/>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="44"/>
       <c r="C46" s="42"/>
       <c r="D46" s="42"/>
@@ -35226,15 +35081,12 @@
       <c r="H46" s="42"/>
       <c r="I46" s="42"/>
       <c r="J46" s="42"/>
-      <c r="K46" s="47"/>
-      <c r="L46" s="48"/>
-    </row>
-    <row r="47" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K46" s="42"/>
+    </row>
+    <row r="47" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="43"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="46"/>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="44"/>
       <c r="C48" s="42"/>
       <c r="D48" s="42"/>
@@ -35244,15 +35096,12 @@
       <c r="H48" s="42"/>
       <c r="I48" s="42"/>
       <c r="J48" s="42"/>
-      <c r="K48" s="47"/>
-      <c r="L48" s="48"/>
-    </row>
-    <row r="49" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K48" s="42"/>
+    </row>
+    <row r="49" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="43"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="46"/>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B50" s="44"/>
       <c r="C50" s="42"/>
       <c r="D50" s="42"/>
@@ -35262,15 +35111,12 @@
       <c r="H50" s="42"/>
       <c r="I50" s="42"/>
       <c r="J50" s="42"/>
-      <c r="K50" s="47"/>
-      <c r="L50" s="48"/>
-    </row>
-    <row r="51" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K50" s="42"/>
+    </row>
+    <row r="51" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="43"/>
-      <c r="K51" s="45"/>
-      <c r="L51" s="46"/>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B52" s="44"/>
       <c r="C52" s="42"/>
       <c r="D52" s="42"/>
@@ -35280,15 +35126,12 @@
       <c r="H52" s="42"/>
       <c r="I52" s="42"/>
       <c r="J52" s="42"/>
-      <c r="K52" s="47"/>
-      <c r="L52" s="48"/>
-    </row>
-    <row r="53" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K52" s="42"/>
+    </row>
+    <row r="53" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="43"/>
-      <c r="K53" s="45"/>
-      <c r="L53" s="46"/>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B54" s="44"/>
       <c r="C54" s="42"/>
       <c r="D54" s="42"/>
@@ -35298,15 +35141,12 @@
       <c r="H54" s="42"/>
       <c r="I54" s="42"/>
       <c r="J54" s="42"/>
-      <c r="K54" s="47"/>
-      <c r="L54" s="48"/>
-    </row>
-    <row r="55" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K54" s="42"/>
+    </row>
+    <row r="55" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="43"/>
-      <c r="K55" s="45"/>
-      <c r="L55" s="46"/>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B56" s="44"/>
       <c r="C56" s="42"/>
       <c r="D56" s="42"/>
@@ -35316,15 +35156,12 @@
       <c r="H56" s="42"/>
       <c r="I56" s="42"/>
       <c r="J56" s="42"/>
-      <c r="K56" s="47"/>
-      <c r="L56" s="48"/>
-    </row>
-    <row r="57" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K56" s="42"/>
+    </row>
+    <row r="57" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="43"/>
-      <c r="K57" s="45"/>
-      <c r="L57" s="46"/>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B58" s="44"/>
       <c r="C58" s="42"/>
       <c r="D58" s="42"/>
@@ -35334,15 +35171,12 @@
       <c r="H58" s="42"/>
       <c r="I58" s="42"/>
       <c r="J58" s="42"/>
-      <c r="K58" s="47"/>
-      <c r="L58" s="48"/>
-    </row>
-    <row r="59" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K58" s="42"/>
+    </row>
+    <row r="59" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="43"/>
-      <c r="K59" s="45"/>
-      <c r="L59" s="46"/>
-    </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B60" s="44"/>
       <c r="C60" s="42"/>
       <c r="D60" s="42"/>
@@ -35352,15 +35186,12 @@
       <c r="H60" s="42"/>
       <c r="I60" s="42"/>
       <c r="J60" s="42"/>
-      <c r="K60" s="47"/>
-      <c r="L60" s="48"/>
-    </row>
-    <row r="61" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K60" s="42"/>
+    </row>
+    <row r="61" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="43"/>
-      <c r="K61" s="45"/>
-      <c r="L61" s="46"/>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B62" s="44"/>
       <c r="C62" s="42"/>
       <c r="D62" s="42"/>
@@ -35370,15 +35201,12 @@
       <c r="H62" s="42"/>
       <c r="I62" s="42"/>
       <c r="J62" s="42"/>
-      <c r="K62" s="47"/>
-      <c r="L62" s="48"/>
-    </row>
-    <row r="63" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K62" s="42"/>
+    </row>
+    <row r="63" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="43"/>
-      <c r="K63" s="45"/>
-      <c r="L63" s="46"/>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B64" s="44"/>
       <c r="C64" s="42"/>
       <c r="D64" s="42"/>
@@ -35388,15 +35216,12 @@
       <c r="H64" s="42"/>
       <c r="I64" s="42"/>
       <c r="J64" s="42"/>
-      <c r="K64" s="47"/>
-      <c r="L64" s="48"/>
-    </row>
-    <row r="65" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K64" s="42"/>
+    </row>
+    <row r="65" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="43"/>
-      <c r="K65" s="45"/>
-      <c r="L65" s="46"/>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B66" s="44"/>
       <c r="C66" s="42"/>
       <c r="D66" s="42"/>
@@ -35406,15 +35231,12 @@
       <c r="H66" s="42"/>
       <c r="I66" s="42"/>
       <c r="J66" s="42"/>
-      <c r="K66" s="47"/>
-      <c r="L66" s="48"/>
-    </row>
-    <row r="67" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K66" s="42"/>
+    </row>
+    <row r="67" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="43"/>
-      <c r="K67" s="45"/>
-      <c r="L67" s="46"/>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B68" s="44"/>
       <c r="C68" s="42"/>
       <c r="D68" s="42"/>
@@ -35424,15 +35246,12 @@
       <c r="H68" s="42"/>
       <c r="I68" s="42"/>
       <c r="J68" s="42"/>
-      <c r="K68" s="47"/>
-      <c r="L68" s="48"/>
-    </row>
-    <row r="69" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K68" s="42"/>
+    </row>
+    <row r="69" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="43"/>
-      <c r="K69" s="45"/>
-      <c r="L69" s="46"/>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B70" s="44"/>
       <c r="C70" s="42"/>
       <c r="D70" s="42"/>
@@ -35442,15 +35261,12 @@
       <c r="H70" s="42"/>
       <c r="I70" s="42"/>
       <c r="J70" s="42"/>
-      <c r="K70" s="47"/>
-      <c r="L70" s="48"/>
-    </row>
-    <row r="71" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K70" s="42"/>
+    </row>
+    <row r="71" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="43"/>
-      <c r="K71" s="45"/>
-      <c r="L71" s="46"/>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B72" s="44"/>
       <c r="C72" s="42"/>
       <c r="D72" s="42"/>
@@ -35460,15 +35276,12 @@
       <c r="H72" s="42"/>
       <c r="I72" s="42"/>
       <c r="J72" s="42"/>
-      <c r="K72" s="47"/>
-      <c r="L72" s="48"/>
-    </row>
-    <row r="73" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K72" s="42"/>
+    </row>
+    <row r="73" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="43"/>
-      <c r="K73" s="45"/>
-      <c r="L73" s="46"/>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B74" s="44"/>
       <c r="C74" s="42"/>
       <c r="D74" s="42"/>
@@ -35478,15 +35291,12 @@
       <c r="H74" s="42"/>
       <c r="I74" s="42"/>
       <c r="J74" s="42"/>
-      <c r="K74" s="47"/>
-      <c r="L74" s="48"/>
-    </row>
-    <row r="75" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K74" s="42"/>
+    </row>
+    <row r="75" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="43"/>
-      <c r="K75" s="45"/>
-      <c r="L75" s="46"/>
-    </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B76" s="44"/>
       <c r="C76" s="42"/>
       <c r="D76" s="42"/>
@@ -35496,15 +35306,12 @@
       <c r="H76" s="42"/>
       <c r="I76" s="42"/>
       <c r="J76" s="42"/>
-      <c r="K76" s="47"/>
-      <c r="L76" s="48"/>
-    </row>
-    <row r="77" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K76" s="42"/>
+    </row>
+    <row r="77" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="43"/>
-      <c r="K77" s="45"/>
-      <c r="L77" s="46"/>
-    </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B78" s="44"/>
       <c r="C78" s="42"/>
       <c r="D78" s="42"/>
@@ -35514,15 +35321,12 @@
       <c r="H78" s="42"/>
       <c r="I78" s="42"/>
       <c r="J78" s="42"/>
-      <c r="K78" s="47"/>
-      <c r="L78" s="48"/>
-    </row>
-    <row r="79" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K78" s="42"/>
+    </row>
+    <row r="79" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="43"/>
-      <c r="K79" s="45"/>
-      <c r="L79" s="46"/>
-    </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B80" s="44"/>
       <c r="C80" s="42"/>
       <c r="D80" s="42"/>
@@ -35532,17 +35336,15 @@
       <c r="H80" s="42"/>
       <c r="I80" s="42"/>
       <c r="J80" s="42"/>
-      <c r="K80" s="47"/>
-      <c r="L80" s="48"/>
+      <c r="K80" s="42"/>
     </row>
   </sheetData>
   <sheetProtection objects="1" scenarios="1"/>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="F8:G8"/>
-    <mergeCell ref="K13:L13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
kinerja amt bisa lebih dari satu dalam sehari
</commit_message>
<xml_diff>
--- a/coba - Copy.xlsx
+++ b/coba - Copy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19020" windowHeight="9345" tabRatio="961" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19020" windowHeight="9345" tabRatio="961" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Operasi Harian" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2557" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="603">
   <si>
     <t>PT. Patra Niaga</t>
   </si>
@@ -8385,7 +8385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -34553,8 +34553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -34864,16 +34864,36 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="44"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
+      <c r="B18" s="43">
+        <v>41883</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>602</v>
+      </c>
+      <c r="D18" t="s">
+        <v>463</v>
+      </c>
+      <c r="E18" t="s">
+        <v>454</v>
+      </c>
+      <c r="F18" t="s">
+        <v>476</v>
+      </c>
+      <c r="G18">
+        <v>16</v>
+      </c>
+      <c r="H18">
+        <v>177</v>
+      </c>
+      <c r="I18">
+        <v>64</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="43"/>

</xml_diff>